<commit_message>
Updated layout and ran ERC
</commit_message>
<xml_diff>
--- a/Elekid-MCU/Project Outputs for Elekid_MCU/BOM/Bill of Materials-Elekid_MCU.xlsx
+++ b/Elekid-MCU/Project Outputs for Elekid_MCU/BOM/Bill of Materials-Elekid_MCU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MinYoung Park\Documents\GitHub\electrical-Embedded\Elekid-MCU\Project Outputs for Elekid_MCU\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FC63F2-D3F5-43AA-8490-F769C663EB13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44EDB922-2BA4-4051-855C-7C9B7CDD2FFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{0FD97C15-D16E-4307-B258-1F2F3259761B}"/>
+    <workbookView xWindow="14025" yWindow="-165" windowWidth="14400" windowHeight="10875" xr2:uid="{3833BA02-C5A8-4095-A143-63F1488C86AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Elekid_MCU" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Designator</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>B4B-XH</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>HDR1X5</t>
   </si>
   <si>
     <t>R1, R2, R3, R4</t>
@@ -595,15 +601,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9314F8-249F-446C-91C4-875DDE55A00A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDD50D3-E5E7-4449-A509-A0B96197A578}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -838,42 +842,42 @@
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="4">
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="4">
         <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -892,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
@@ -900,85 +904,101 @@
       <c r="C14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="H15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="H16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="4">
+      <c r="B18" s="4"/>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>